<commit_message>
Fixed taxes and line charge calculations, and changed a bit of formatting.
</commit_message>
<xml_diff>
--- a/Ting Bill Splitter.xlsx
+++ b/Ting Bill Splitter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefano\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefano\git\TingBillSplitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Month" sheetId="1" r:id="rId1"/>
     <sheet name="Minutes" sheetId="2" r:id="rId2"/>
     <sheet name="Messages" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Megabytes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t>Minutes Used</t>
-  </si>
-  <si>
-    <t>SMS Used</t>
-  </si>
-  <si>
-    <t>Data Used</t>
   </si>
   <si>
     <t>Cost for Minutes</t>
@@ -110,9 +104,6 @@
     <t>Override</t>
   </si>
   <si>
-    <t>May Ting Bill</t>
-  </si>
-  <si>
     <t>Created by Stefano Prezioso</t>
   </si>
   <si>
@@ -122,19 +113,29 @@
     <t>Paste Entire Messages Spreadsheet Here</t>
   </si>
   <si>
-    <t>Paste Entire Data Spreadsheet Here</t>
+    <t>Paste Entire Megabytes Spreadsheet Here</t>
+  </si>
+  <si>
+    <t>Megabytes Used</t>
+  </si>
+  <si>
+    <t>Messages Used</t>
+  </si>
+  <si>
+    <t>Ting Bill Breakdown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00_ ;\-[$$-409]#,##0.00\ "/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.000;[Red]&quot;$&quot;#,##0.000"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.0000;[Red]&quot;$&quot;#,##0.0000"/>
+    <numFmt numFmtId="169" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -341,7 +342,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -387,7 +388,13 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -402,15 +409,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -837,7 +839,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -846,20 +848,21 @@
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="A1" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -884,37 +887,37 @@
         <v>3</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="8" t="e">
         <f>L3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="5">
         <f>SUMIF(Minutes!$D$2:$D$7500, $C3, Minutes!$L$2:$L$7500)</f>
         <v>0</v>
@@ -924,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="6">
-        <f>(SUMIF(Data!$B$2:$B$7500, $C3, Data!$D$2:$D$7500))/1024</f>
+        <f>(SUMIF(Megabytes!$B$2:$B$7500, $C3, Megabytes!$D$2:$D$7500))/1024</f>
         <v>0</v>
       </c>
       <c r="G3" s="8" t="e">
@@ -940,10 +943,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J3" s="8">
-        <v>6</v>
-      </c>
-      <c r="K3" s="8">
-        <f>$B$13/5</f>
+        <f>IF(ISBLANK(C3), 0, 6)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="37">
+        <f t="shared" ref="K3:K6" si="0">IF(ISBLANK(C3), 0, $B$13/($J$8/6))</f>
         <v>0</v>
       </c>
       <c r="L3" s="8" t="e">
@@ -952,12 +956,12 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="9" t="e">
-        <f t="shared" ref="B4:B7" si="0">L4</f>
+        <f t="shared" ref="B4:B7" si="1">L4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="5">
         <f>SUMIF(Minutes!$D$2:$D$7500, $C4, Minutes!$L$2:$L$7500)</f>
         <v>0</v>
@@ -967,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <f>(SUMIF(Data!$B$2:$B$7500, $C4, Data!$D$2:$D$7500))/1024</f>
+        <f>(SUMIF(Megabytes!$B$2:$B$7500, $C4, Megabytes!$D$2:$D$7500))/1024</f>
         <v>0</v>
       </c>
       <c r="G4" s="9" t="e">
@@ -982,25 +986,26 @@
         <f>(F4/SUM($F$3:$F$7))*$B$12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J4" s="9">
-        <v>6</v>
-      </c>
-      <c r="K4" s="9">
-        <f>$B$13/5</f>
+      <c r="J4" s="8">
+        <f t="shared" ref="J4:J7" si="2">IF(ISBLANK(C4), 0, 6)</f>
         <v>0</v>
       </c>
+      <c r="K4" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L4" s="9" t="e">
-        <f t="shared" ref="L4:L7" si="1">SUM(G4:K4)</f>
+        <f t="shared" ref="L4:L7" si="3">SUM(G4:K4)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="9" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="5">
         <f>SUMIF(Minutes!$D$2:$D$7500, $C5, Minutes!$L$2:$L$7500)</f>
         <v>0</v>
@@ -1010,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <f>(SUMIF(Data!$B$2:$B$7500, $C5, Data!$D$2:$D$7500))/1024</f>
+        <f>(SUMIF(Megabytes!$B$2:$B$7500, $C5, Megabytes!$D$2:$D$7500))/1024</f>
         <v>0</v>
       </c>
       <c r="G5" s="9" t="e">
@@ -1025,25 +1030,26 @@
         <f>(F5/SUM($F$3:$F$7))*$B$12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J5" s="9">
-        <v>6</v>
-      </c>
-      <c r="K5" s="9">
-        <f>$B$13/5</f>
+      <c r="J5" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K5" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L5" s="9" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="9" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="5">
         <f>SUMIF(Minutes!$D$2:$D$7500, $C6, Minutes!$L$2:$L$7500)</f>
         <v>0</v>
@@ -1053,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="4">
-        <f>(SUMIF(Data!$B$2:$B$7500, $C6, Data!$D$2:$D$7500))/1024</f>
+        <f>(SUMIF(Megabytes!$B$2:$B$7500, $C6, Megabytes!$D$2:$D$7500))/1024</f>
         <v>0</v>
       </c>
       <c r="G6" s="9" t="e">
@@ -1068,25 +1074,26 @@
         <f>(F6/SUM($F$3:$F$7))*$B$12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J6" s="9">
-        <v>6</v>
-      </c>
-      <c r="K6" s="9">
-        <f>$B$13/5</f>
+      <c r="J6" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K6" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L6" s="9" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="9" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="5">
         <f>SUMIF(Minutes!$D$2:$D$7500, $C7, Minutes!$L$2:$L$7500)</f>
         <v>0</v>
@@ -1096,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <f>(SUMIF(Data!$B$2:$B$7500, $C7, Data!$D$2:$D$7500))/1024</f>
+        <f>(SUMIF(Megabytes!$B$2:$B$7500, $C7, Megabytes!$D$2:$D$7500))/1024</f>
         <v>0</v>
       </c>
       <c r="G7" s="9" t="e">
@@ -1111,15 +1118,16 @@
         <f>(F7/SUM($F$3:$F$7))*$B$12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7" s="9">
-        <v>6</v>
-      </c>
-      <c r="K7" s="9">
-        <f>$B$13/5</f>
+      <c r="J7" s="8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K7" s="37">
+        <f>IF(ISBLANK(C7), 0, $B$13/($J$8/6))</f>
+        <v>0</v>
+      </c>
       <c r="L7" s="9" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1129,11 +1137,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="11">
-        <f t="shared" ref="E8:F8" si="2">SUM(E3:E7)</f>
+        <f t="shared" ref="E8:F8" si="4">SUM(E3:E7)</f>
         <v>0</v>
       </c>
       <c r="F8" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G8" s="10" t="e">
@@ -1141,19 +1149,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H8" s="10" t="e">
-        <f t="shared" ref="H8:K8" si="3">SUM(H3:H7)</f>
+        <f t="shared" ref="H8:K8" si="5">SUM(H3:H7)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I8" s="10" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J8" s="10">
-        <f t="shared" si="3"/>
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="K8" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L8" s="10" t="e">
@@ -1162,28 +1170,28 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="str">
+      <c r="A9" s="36" t="str">
         <f>A1</f>
-        <v>May Ting Bill</v>
-      </c>
-      <c r="B9" s="25"/>
+        <v>Ting Bill Breakdown</v>
+      </c>
+      <c r="B9" s="36"/>
       <c r="C9" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="20">
         <f>IF(ISBLANK(C10),IF(D8=0, 0,(IF(D8&lt;=C17,C18, IF(D8&lt;=D17,D18, IF(D8&lt;=E17,E18, IF(D8&lt;=F17,F18, F18+((D8-F17)*G18))))))), C10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="30"/>
+      <c r="C10" s="25"/>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="20">
         <f>IF(ISBLANK(C11),IF(E8=0, 0, (IF(E8&lt;=C19,C20, IF(E8&lt;=D19,D20, IF(E8&lt;=E19,E20, IF(E8&lt;=F19,F20, F20+((E8-F19)*G20))))))), C11)</f>
@@ -1193,7 +1201,7 @@
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="20">
         <f>IF(ISBLANK(C12),IF(F8=0, 0, (IF(F8&lt;=C21,C22, IF(F8&lt;=D21,D22, IF(F8&lt;=E21,E22, IF(F8&lt;=F21,F22, F22+((F8-F21)*G22))))))), C12)</f>
@@ -1203,42 +1211,42 @@
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" s="21"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="21"/>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="G16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>13</v>
+      <c r="A17" s="32" t="s">
+        <v>11</v>
       </c>
       <c r="B17" s="13">
         <v>0</v>
@@ -1256,11 +1264,11 @@
         <v>2100</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="14">
         <v>0</v>
       </c>
@@ -1281,8 +1289,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>14</v>
+      <c r="A19" s="34" t="s">
+        <v>12</v>
       </c>
       <c r="B19" s="16">
         <v>0</v>
@@ -1300,11 +1308,11 @@
         <v>4800</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="17">
         <v>0</v>
       </c>
@@ -1325,8 +1333,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>15</v>
+      <c r="A21" s="32" t="s">
+        <v>13</v>
       </c>
       <c r="B21" s="13">
         <v>0</v>
@@ -1344,11 +1352,11 @@
         <v>2000</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="14">
         <v>0</v>
       </c>
@@ -1369,10 +1377,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="35"/>
+      <c r="A24" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1433,8 +1441,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>29</v>
+      <c r="A1" s="30" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3035,9 +3043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2282"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3045,8 +3051,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>30</v>
+      <c r="A1" s="30" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -12187,9 +12193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12197,8 +12201,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>31</v>
+      <c r="A1" s="30" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>